<commit_message>
fix time recording variable values
</commit_message>
<xml_diff>
--- a/research_data.xlsx
+++ b/research_data.xlsx
@@ -912,7 +912,7 @@
         <v>14</v>
       </c>
       <c r="V5" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="W5" t="n">
         <v>29</v>
@@ -1006,7 +1006,7 @@
         <v>18</v>
       </c>
       <c r="V6" t="n">
-        <v>1337</v>
+        <v>4</v>
       </c>
       <c r="W6" t="n">
         <v>38</v>
@@ -1097,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="U7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V7" t="n">
         <v>1</v>
@@ -1964,7 +1964,7 @@
         <v>13</v>
       </c>
       <c r="V16" t="n">
-        <v>2654</v>
+        <v>18</v>
       </c>
       <c r="W16" t="n">
         <v>25</v>
@@ -2346,7 +2346,7 @@
         <v>4</v>
       </c>
       <c r="U20" t="n">
-        <v>139</v>
+        <v>15</v>
       </c>
       <c r="V20" t="n">
         <v>24</v>
@@ -3017,7 +3017,7 @@
         <v>3</v>
       </c>
       <c r="U27" t="n">
-        <v>93</v>
+        <v>21</v>
       </c>
       <c r="V27" t="n">
         <v>14</v>
@@ -3115,10 +3115,10 @@
         <v>3</v>
       </c>
       <c r="U28" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="V28" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="W28" t="n">
         <v>20</v>
@@ -3497,7 +3497,7 @@
         <v>2</v>
       </c>
       <c r="U32" t="n">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="V32" t="n">
         <v>9</v>
@@ -3779,7 +3779,7 @@
         <v>2</v>
       </c>
       <c r="U35" t="n">
-        <v>478</v>
+        <v>10</v>
       </c>
       <c r="V35" t="n">
         <v>11</v>
@@ -4452,7 +4452,7 @@
         <v>28</v>
       </c>
       <c r="V42" t="n">
-        <v>319</v>
+        <v>8</v>
       </c>
       <c r="W42" t="n">
         <v>20</v>
@@ -4637,10 +4637,10 @@
         <v>3</v>
       </c>
       <c r="U44" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="V44" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="W44" t="n">
         <v>26</v>
@@ -5026,10 +5026,10 @@
         <v>2</v>
       </c>
       <c r="U48" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="V48" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="W48" t="n">
         <v>25</v>
@@ -5787,7 +5787,7 @@
         <v>5</v>
       </c>
       <c r="U56" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V56" t="n">
         <v>7</v>
@@ -5881,7 +5881,7 @@
         <v>3</v>
       </c>
       <c r="U57" t="n">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="V57" t="n">
         <v>5</v>
@@ -5975,10 +5975,10 @@
         <v>3</v>
       </c>
       <c r="U58" t="n">
-        <v>204</v>
+        <v>19</v>
       </c>
       <c r="V58" t="n">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="W58" t="n">
         <v>35</v>
@@ -6163,7 +6163,7 @@
         <v>4</v>
       </c>
       <c r="U60" t="n">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="V60" t="n">
         <v>35</v>
@@ -6260,7 +6260,7 @@
         <v>3</v>
       </c>
       <c r="U61" t="n">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="V61" t="n">
         <v>24</v>
@@ -6448,10 +6448,10 @@
         <v>4</v>
       </c>
       <c r="U63" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="V63" t="n">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="W63" t="n">
         <v>40</v>
@@ -6918,10 +6918,10 @@
         <v>2</v>
       </c>
       <c r="U68" t="n">
-        <v>987</v>
+        <v>7</v>
       </c>
       <c r="V68" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="W68" t="n">
         <v>39</v>
@@ -7109,10 +7109,10 @@
         <v>3</v>
       </c>
       <c r="U70" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="V70" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="W70" t="n">
         <v>34</v>
@@ -7207,7 +7207,7 @@
         <v>4</v>
       </c>
       <c r="U71" t="n">
-        <v>1386</v>
+        <v>21</v>
       </c>
       <c r="V71" t="n">
         <v>13</v>
@@ -7395,7 +7395,7 @@
         <v>4</v>
       </c>
       <c r="U73" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="V73" t="n">
         <v>1</v>
@@ -7589,7 +7589,7 @@
         <v>19</v>
       </c>
       <c r="V75" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="W75" t="n">
         <v>23</v>
@@ -7685,10 +7685,10 @@
         <v>3</v>
       </c>
       <c r="U76" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="V76" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="W76" t="n">
         <v>21</v>
@@ -7779,10 +7779,10 @@
         <v>4</v>
       </c>
       <c r="U77" t="n">
-        <v>911</v>
+        <v>20</v>
       </c>
       <c r="V77" t="n">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="W77" t="n">
         <v>29</v>
@@ -8249,10 +8249,10 @@
         <v>3</v>
       </c>
       <c r="U82" t="n">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="V82" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="W82" t="n">
         <v>34</v>
@@ -8347,7 +8347,7 @@
         <v>3</v>
       </c>
       <c r="U83" t="n">
-        <v>171</v>
+        <v>20</v>
       </c>
       <c r="V83" t="n">
         <v>14</v>
@@ -8441,10 +8441,10 @@
         <v>3</v>
       </c>
       <c r="U84" t="n">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="V84" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="W84" t="n">
         <v>55</v>
@@ -8535,10 +8535,10 @@
         <v>3</v>
       </c>
       <c r="U85" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="V85" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="W85" t="n">
         <v>24</v>
@@ -8632,7 +8632,7 @@
         <v>13</v>
       </c>
       <c r="V86" t="n">
-        <v>2807</v>
+        <v>19</v>
       </c>
       <c r="W86" t="n">
         <v>26</v>
@@ -8723,7 +8723,7 @@
         <v>2</v>
       </c>
       <c r="U87" t="n">
-        <v>1653</v>
+        <v>20</v>
       </c>
       <c r="V87" t="n">
         <v>5</v>
@@ -8817,7 +8817,7 @@
         <v>3</v>
       </c>
       <c r="U88" t="n">
-        <v>282</v>
+        <v>17</v>
       </c>
       <c r="V88" t="n">
         <v>8</v>
@@ -9204,7 +9204,7 @@
         <v>3</v>
       </c>
       <c r="U92" t="n">
-        <v>223</v>
+        <v>61</v>
       </c>
       <c r="V92" t="n">
         <v>10</v>
@@ -9779,10 +9779,10 @@
         <v>3</v>
       </c>
       <c r="U98" t="n">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="V98" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="W98" t="n">
         <v>36</v>
@@ -10065,7 +10065,7 @@
         <v>3</v>
       </c>
       <c r="U101" t="n">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="V101" t="n">
         <v>19</v>
@@ -10546,7 +10546,7 @@
         <v>3</v>
       </c>
       <c r="U106" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="V106" t="n">
         <v>13</v>
@@ -11413,7 +11413,7 @@
         <v>12</v>
       </c>
       <c r="V115" t="n">
-        <v>190</v>
+        <v>23</v>
       </c>
       <c r="W115" t="n">
         <v>26</v>
@@ -11699,7 +11699,7 @@
         <v>3</v>
       </c>
       <c r="U118" t="n">
-        <v>1797</v>
+        <v>20</v>
       </c>
       <c r="V118" t="n">
         <v>9</v>
@@ -11890,7 +11890,7 @@
         <v>3</v>
       </c>
       <c r="U120" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="V120" t="n">
         <v>3</v>
@@ -12182,7 +12182,7 @@
         <v>3</v>
       </c>
       <c r="U123" t="n">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="V123" t="n">
         <v>20</v>
@@ -12850,7 +12850,7 @@
         <v>7</v>
       </c>
       <c r="U130" t="n">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="V130" t="n">
         <v>6</v>
@@ -14004,7 +14004,7 @@
         <v>3</v>
       </c>
       <c r="U142" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="V142" t="n">
         <v>8</v>
@@ -14290,10 +14290,10 @@
         <v>2</v>
       </c>
       <c r="U145" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="V145" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="W145" t="n">
         <v>27</v>
@@ -14951,10 +14951,10 @@
         <v>3</v>
       </c>
       <c r="U152" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="V152" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="W152" t="n">
         <v>29</v>
@@ -15045,7 +15045,7 @@
         <v>3</v>
       </c>
       <c r="U153" t="n">
-        <v>3080</v>
+        <v>13</v>
       </c>
       <c r="V153" t="n">
         <v>32</v>
@@ -15341,7 +15341,7 @@
         <v>3</v>
       </c>
       <c r="U156" t="n">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="V156" t="n">
         <v>50</v>
@@ -15529,10 +15529,10 @@
         <v>2</v>
       </c>
       <c r="U158" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W158" t="n">
         <v>2</v>
@@ -15635,7 +15635,7 @@
         <v>2</v>
       </c>
       <c r="U159" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="V159" t="n">
         <v>8</v>
@@ -15921,10 +15921,10 @@
         <v>2</v>
       </c>
       <c r="U162" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="V162" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="W162" t="n">
         <v>28</v>
@@ -16018,7 +16018,7 @@
         <v>2</v>
       </c>
       <c r="U163" t="n">
-        <v>3080</v>
+        <v>0</v>
       </c>
       <c r="V163" t="n">
         <v>13</v>
@@ -16397,7 +16397,7 @@
         <v>3</v>
       </c>
       <c r="U167" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="V167" t="n">
         <v>4</v>
@@ -16491,10 +16491,10 @@
         <v>3</v>
       </c>
       <c r="U168" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="V168" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="W168" t="n">
         <v>10</v>
@@ -17159,7 +17159,7 @@
         <v>4</v>
       </c>
       <c r="U175" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V175" t="n">
         <v>4</v>
@@ -17350,7 +17350,7 @@
         <v>2</v>
       </c>
       <c r="U177" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V177" t="n">
         <v>5</v>
@@ -17830,10 +17830,10 @@
         <v>5</v>
       </c>
       <c r="U182" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="V182" t="n">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="W182" t="n">
         <v>59</v>
@@ -18024,7 +18024,7 @@
         <v>3</v>
       </c>
       <c r="U184" t="n">
-        <v>961</v>
+        <v>33</v>
       </c>
       <c r="V184" t="n">
         <v>24</v>
@@ -18122,7 +18122,7 @@
         <v>3</v>
       </c>
       <c r="U185" t="n">
-        <v>912</v>
+        <v>29</v>
       </c>
       <c r="V185" t="n">
         <v>51</v>
@@ -18216,10 +18216,10 @@
         <v>4</v>
       </c>
       <c r="U186" t="n">
-        <v>1131</v>
+        <v>3</v>
       </c>
       <c r="V186" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="W186" t="n">
         <v>9</v>
@@ -18315,7 +18315,7 @@
         <v>3</v>
       </c>
       <c r="U187" t="n">
-        <v>284</v>
+        <v>7</v>
       </c>
       <c r="V187" t="n">
         <v>6</v>
@@ -18898,10 +18898,10 @@
         <v>5</v>
       </c>
       <c r="U193" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="V193" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="W193" t="n">
         <v>24</v>
@@ -18994,7 +18994,7 @@
         <v>3</v>
       </c>
       <c r="U194" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="V194" t="n">
         <v>6</v>
@@ -19285,10 +19285,10 @@
         <v>3</v>
       </c>
       <c r="U197" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="V197" t="n">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="W197" t="n">
         <v>17</v>
@@ -19858,7 +19858,7 @@
         <v>3</v>
       </c>
       <c r="U203" t="n">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="V203" t="n">
         <v>5</v>
@@ -20145,10 +20145,10 @@
         <v>3</v>
       </c>
       <c r="U206" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="V206" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="W206" t="n">
         <v>25</v>
@@ -20430,7 +20430,7 @@
         <v>3</v>
       </c>
       <c r="U209" t="n">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="V209" t="n">
         <v>19</v>
@@ -20916,7 +20916,7 @@
         <v>20</v>
       </c>
       <c r="V214" t="n">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="W214" t="n">
         <v>34</v>
@@ -21673,7 +21673,7 @@
         <v>3</v>
       </c>
       <c r="U222" t="n">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="V222" t="n">
         <v>9</v>
@@ -21771,7 +21771,7 @@
         <v>3</v>
       </c>
       <c r="U223" t="n">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="V223" t="n">
         <v>12</v>
@@ -22256,10 +22256,10 @@
         <v>3</v>
       </c>
       <c r="U228" t="n">
-        <v>504</v>
+        <v>0</v>
       </c>
       <c r="V228" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="W228" t="n">
         <v>26</v>
@@ -22827,7 +22827,7 @@
         <v>4</v>
       </c>
       <c r="U234" t="n">
-        <v>397</v>
+        <v>22</v>
       </c>
       <c r="V234" t="n">
         <v>12</v>
@@ -23117,7 +23117,7 @@
         <v>3</v>
       </c>
       <c r="U237" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="V237" t="n">
         <v>5</v>
@@ -24545,7 +24545,7 @@
         <v>2</v>
       </c>
       <c r="U252" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="V252" t="n">
         <v>3</v>
@@ -24642,7 +24642,7 @@
         <v>23</v>
       </c>
       <c r="V253" t="n">
-        <v>217</v>
+        <v>30</v>
       </c>
       <c r="W253" t="n">
         <v>22</v>

</xml_diff>